<commit_message>
add alternatif siswa & import
</commit_message>
<xml_diff>
--- a/public/templates/template_alternatif_siswa.xlsx
+++ b/public/templates/template_alternatif_siswa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilham\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\web_rangking\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD23252E-1CEC-4616-B00F-AECC89389658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A636B3B-DCD0-4F66-98FC-2A99A450582C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="9468" xr2:uid="{94A31312-417A-4387-8D13-51378609E6A9}"/>
+    <workbookView xWindow="-22416" yWindow="3600" windowWidth="17280" windowHeight="9468" xr2:uid="{94A31312-417A-4387-8D13-51378609E6A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>prestasi_non_akademik</t>
   </si>
   <si>
-    <t>jumlah_pelanggaran_tt_displin</t>
+    <t>jumlah_pelanggaran_tt_disiplin</t>
   </si>
 </sst>
 </file>
@@ -128,24 +128,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,117 +460,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04301CC0-A2F1-40FC-A001-C574080DA2DD}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="40.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="43.77734375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add konversi fuzzy function
</commit_message>
<xml_diff>
--- a/public/templates/template_alternatif_siswa.xlsx
+++ b/public/templates/template_alternatif_siswa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\web_rangking\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A636B3B-DCD0-4F66-98FC-2A99A450582C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4337D7B-4E71-4568-956A-B60AE98EB3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22416" yWindow="3600" windowWidth="17280" windowHeight="9468" xr2:uid="{94A31312-417A-4387-8D13-51378609E6A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{94A31312-417A-4387-8D13-51378609E6A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>nama_siswa</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>jumlah_pelanggaran_tt_disiplin</t>
+  </si>
+  <si>
+    <t>kode_siswa</t>
   </si>
 </sst>
 </file>
@@ -458,117 +461,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04301CC0-A2F1-40FC-A001-C574080DA2DD}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="43.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="4"/>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I3" s="6"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I4" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I5" s="6"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I6" s="6"/>
+      <c r="L5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I7" s="6"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I8" s="6"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I10" s="6"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="4"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="6"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I12" s="6"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="6"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I14" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I15" s="6"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="4"/>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="4"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="4"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="4"/>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H64" s="4"/>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="4"/>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="4"/>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="4"/>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="I3:K8"/>
-    <mergeCell ref="I10:K15"/>
+    <mergeCell ref="J3:L8"/>
+    <mergeCell ref="J10:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>